<commit_message>
DMS: Fix KpiProductGrouping Template
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Product_Grouping.xlsx
+++ b/DMS/Templates/Kpi_Product_Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dotNet\DMS\DMS.BE\DMS\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12557C00-DEC9-4694-841E-3701FAB6FDDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5C17BE-C648-47BE-948D-F925A1EC8CA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,9 +60,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
-  <si>
-    <t>THIẾT LẬP KPI SẢN PHẨM</t>
-  </si>
   <si>
     <t>Kỳ</t>
   </si>
@@ -176,6 +173,9 @@
   <si>
     <t>{{ProductGroupings.Name}}</t>
   </si>
+  <si>
+    <t>THIẾT LẬP KPI NHÓM SẢN PHẨM</t>
+  </si>
 </sst>
 </file>
 
@@ -234,7 +234,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +275,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FFD9E2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -321,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -344,12 +350,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +579,7 @@
   <dimension ref="A1:G998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -585,23 +593,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
@@ -611,33 +619,33 @@
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -647,23 +655,23 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -2358,12 +2366,15 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"2020.0,2021.0,2022.0,2023.0,2024.0,2025.0,2026.0,2027.0,2028.0,2029.0,2030.0"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C355" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"KPI nhóm sản phẩm mới,KPI nhóm sản phẩm trọng tâm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{A9BB55B2-97F6-4387-BC3D-4F6999F0848B}">
+      <formula1>"Tháng 1, Tháng 2, Tháng 3, Tháng 4, Tháng 5, Tháng 6, Tháng 7, Tháng 8, Tháng 9, Tháng 10, Tháng 11, Tháng 12, Quý 1, Quý 2, Quý 3, Quý 4, Năm"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -2389,18 +2400,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3408,30 +3419,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5111,30 +5122,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6137,7 +6148,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="392.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DMS: Update KpiProductGrouping Template
</commit_message>
<xml_diff>
--- a/DMS/Templates/Kpi_Product_Grouping.xlsx
+++ b/DMS/Templates/Kpi_Product_Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nhungle/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54A5E0E-53B8-EA48-8BC1-59A4414BE8F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393164CE-6A23-1F40-B440-A49661F7CC47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,11 +39,22 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>Các mã sản phẩm cách nhau bằng dấu ";"</t>
+          <t xml:space="preserve">Các mã sản phẩm cách nhau bằng dấu ";"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Mã sản phẩm cuối cùng không được để dấu ";" ở sau
+</t>
         </r>
       </text>
     </comment>
@@ -87,9 +98,6 @@
   </si>
   <si>
     <t>END</t>
-  </si>
-  <si>
-    <t>Vui lòng insert các mã nhóm sản phẩm, mã sản phẩm vào theo từng nhân viên</t>
   </si>
   <si>
     <t>Tên nhóm sản phẩm</t>
@@ -176,6 +184,9 @@
   <si>
     <t>THIẾT LẬP KPI NHÓM SẢN PHẨM</t>
   </si>
+  <si>
+    <t>Vui lòng chọn loại KPI nhóm sản phẩm; insert các mã nhóm sản phẩm, mã sản phẩm và điền số chỉ tiêu KPI vào theo từng nhân viên</t>
+  </si>
 </sst>
 </file>
 
@@ -185,7 +196,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +256,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -597,13 +614,13 @@
   <dimension ref="A1:G998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
     <col min="4" max="5" width="27.5" customWidth="1"/>
     <col min="6" max="7" width="26.6640625" customWidth="1"/>
@@ -612,7 +629,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -659,10 +676,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -671,11 +688,11 @@
       <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>14</v>
+      <c r="A6" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -688,7 +705,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -2420,15 +2437,15 @@
         <v>5</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3439,27 +3456,27 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5142,27 +5159,27 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6165,7 +6182,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="392.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>